<commit_message>
Previous exploration into population and mortality
</commit_message>
<xml_diff>
--- a/data/population+mortality.xlsx
+++ b/data/population+mortality.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\WCA\ons-stats\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F819680-7EE5-465F-B7A7-DCD7DF609651}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFEE5350-9D0F-4546-AA08-5104007AA7A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="6" xr2:uid="{F1DC00DB-4C24-4153-8850-A4055601A7B8}"/>
+    <workbookView xWindow="-24120" yWindow="4740" windowWidth="24240" windowHeight="13740" activeTab="4" xr2:uid="{F1DC00DB-4C24-4153-8850-A4055601A7B8}"/>
   </bookViews>
   <sheets>
     <sheet name="2016" sheetId="1" r:id="rId1"/>
@@ -12534,7 +12534,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15499,11 +15499,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A94A7BF2-66EE-4B1D-8D93-C598B6390EEF}">
   <dimension ref="A1:IU35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="BF2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="CN33" sqref="CN33"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26598,11 +26598,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97F2F032-3C6D-43EB-A753-ED43B41A2301}">
   <dimension ref="A1:BD50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A49" sqref="A49"/>
+      <selection pane="bottomRight" activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>